<commit_message>
mssql ve oracle account eklemeleri tamam
</commit_message>
<xml_diff>
--- a/data/btmigrate_work.xlsx
+++ b/data/btmigrate_work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EnesPekdas\Desktop\Projeler\BT-THY\Otomasyon\BTMigrate\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128C7B17-F98F-495A-B843-D3B754805E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F034C2-3C61-4A71-BBD0-ADCE2563EFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1650" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>PamEnvanterSatır</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>E_YARDIMCI</t>
+  </si>
+  <si>
+    <t>quasys.com</t>
   </si>
 </sst>
 </file>
@@ -528,7 +531,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +620,7 @@
         <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
smart rule eklemeleri düzenlemeleri mevcuttaysa yenilerini üzerine ekleyip güncellemeleri tmaam
</commit_message>
<xml_diff>
--- a/data/btmigrate_work.xlsx
+++ b/data/btmigrate_work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EnesPekdas\Desktop\Projeler\BT-THY\Otomasyon\BTMigrate\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F034C2-3C61-4A71-BBD0-ADCE2563EFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661D36D0-31A0-4C94-A545-18125AA8EA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1650" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="btmigrate_work" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="58">
   <si>
     <t>PamEnvanterSatır</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>quasys.com</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>winscp</t>
   </si>
 </sst>
 </file>
@@ -528,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,6 +607,9 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
       <c r="F2" t="s">
         <v>50</v>
       </c>
@@ -792,6 +801,207 @@
         <v>35</v>
       </c>
       <c r="K7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
application atamaları vs de tamam
</commit_message>
<xml_diff>
--- a/data/btmigrate_work.xlsx
+++ b/data/btmigrate_work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EnesPekdas\Desktop\Projeler\BT-THY\Otomasyon\BTMigrate\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661D36D0-31A0-4C94-A545-18125AA8EA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C113C40-B833-42AD-A1AE-B43E580C888F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
   <si>
     <t>PamEnvanterSatır</t>
   </si>
@@ -188,13 +188,13 @@
     <t>E_YARDIMCI</t>
   </si>
   <si>
-    <t>quasys.com</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>winscp</t>
+    <t>winscp,mssql</t>
+  </si>
+  <si>
+    <t>oracle,winscp</t>
   </si>
 </sst>
 </file>
@@ -534,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +546,7 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -608,7 +608,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
         <v>50</v>
@@ -629,7 +629,7 @@
         <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -786,7 +786,7 @@
         <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
         <v>32</v>
@@ -809,7 +809,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
@@ -838,37 +838,31 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="L9" t="s">
         <v>20</v>
@@ -879,19 +873,22 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -908,37 +905,34 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="K11" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -946,7 +940,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -961,7 +955,7 @@
         <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="I12" t="s">
         <v>34</v>
@@ -970,38 +964,6 @@
         <v>35</v>
       </c>
       <c r="K12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
uçtan uca tamam mssql de linkleme yapılacak sadece
</commit_message>
<xml_diff>
--- a/data/btmigrate_work.xlsx
+++ b/data/btmigrate_work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EnesPekdas\Desktop\Projeler\BT-THY\Otomasyon\BTMigrate\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C113C40-B833-42AD-A1AE-B43E580C888F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF69BF37-9E2F-4734-8BB5-CD0FC1E7DBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="btmigrate_work" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="60">
   <si>
     <t>PamEnvanterSatır</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>oracle,winscp</t>
+  </si>
+  <si>
+    <t>quasys.com</t>
+  </si>
+  <si>
+    <t>S_OZCAN,E_PEKDAS</t>
   </si>
 </sst>
 </file>
@@ -537,7 +543,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +555,7 @@
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -629,7 +635,7 @@
         <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -690,7 +696,7 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
@@ -724,6 +730,9 @@
       <c r="G5" t="s">
         <v>28</v>
       </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
       <c r="I5" t="s">
         <v>17</v>
       </c>
@@ -794,6 +803,9 @@
       <c r="G7" t="s">
         <v>33</v>
       </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
       <c r="I7" t="s">
         <v>34</v>
       </c>
@@ -802,6 +814,9 @@
       </c>
       <c r="K7" t="s">
         <v>32</v>
+      </c>
+      <c r="L7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -826,6 +841,9 @@
       <c r="G8" t="s">
         <v>33</v>
       </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
       <c r="I8" t="s">
         <v>34</v>
       </c>
@@ -834,6 +852,9 @@
       </c>
       <c r="K8" t="s">
         <v>32</v>
+      </c>
+      <c r="L8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -855,6 +876,9 @@
       <c r="G9" t="s">
         <v>51</v>
       </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
       <c r="I9" t="s">
         <v>17</v>
       </c>
@@ -925,6 +949,9 @@
       <c r="G11" t="s">
         <v>16</v>
       </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
       <c r="I11" t="s">
         <v>34</v>
       </c>
@@ -955,6 +982,9 @@
         <v>32</v>
       </c>
       <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
         <v>51</v>
       </c>
       <c r="I12" t="s">

</xml_diff>

<commit_message>
Managed System Loglama oki
</commit_message>
<xml_diff>
--- a/data/btmigrate_work.xlsx
+++ b/data/btmigrate_work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EnesPekdas\Desktop\Projeler\BT-THY\Otomasyon\BTMigrate\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF69BF37-9E2F-4734-8BB5-CD0FC1E7DBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9E686E-1080-4CFE-9E54-B4B57E40AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="btmigrate_work" sheetId="1" r:id="rId1"/>
@@ -197,10 +197,10 @@
     <t>oracle,winscp</t>
   </si>
   <si>
+    <t>S_OZCAN,E_PEKDAS</t>
+  </si>
+  <si>
     <t>quasys.com</t>
-  </si>
-  <si>
-    <t>S_OZCAN,E_PEKDAS</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +635,7 @@
         <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -696,7 +696,7 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
group smart rule verme tamma
</commit_message>
<xml_diff>
--- a/data/btmigrate_work.xlsx
+++ b/data/btmigrate_work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EnesPekdas\Desktop\Projeler\BT-THY\Otomasyon\BTMigrate\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81F5FA5-C52F-4016-AE3E-BBC38F7939B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A6E309-1536-4C1E-966A-9C0125128F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="btmigrate_work" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="57">
   <si>
     <t>PamEnvanterSatır</t>
   </si>
@@ -92,9 +92,6 @@
     <t>10.58.59.104</t>
   </si>
   <si>
-    <t>Server4</t>
-  </si>
-  <si>
     <t>10.58.59.108</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
     <t>1433</t>
   </si>
   <si>
+    <t>thynet.thy.com</t>
+  </si>
+  <si>
     <t>10.58.59.109</t>
   </si>
   <si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>10.58.59.105</t>
+  </si>
+  <si>
+    <t>Server5</t>
   </si>
   <si>
     <t>Y_UCUNCUOGLU</t>
@@ -531,24 +534,10 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -660,7 +649,7 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -689,13 +678,13 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
@@ -704,10 +693,10 @@
         <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L5" t="s">
         <v>18</v>
@@ -727,7 +716,7 @@
         <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
@@ -736,13 +725,13 @@
         <v>17</v>
       </c>
       <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
         <v>27</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -756,13 +745,13 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K7" t="s">
         <v>11</v>
@@ -779,10 +768,10 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -791,13 +780,13 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K8" t="s">
         <v>11</v>
       </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -809,20 +798,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -832,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -841,10 +819,10 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -855,16 +833,16 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -878,19 +856,19 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -901,19 +879,19 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -921,22 +899,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -944,22 +922,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
         <v>50</v>
       </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -967,22 +945,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -990,22 +968,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1013,22 +991,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1036,22 +1014,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
         <v>50</v>
       </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1059,22 +1037,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>